<commit_message>
Removed columns for depth, elevation, and altitude since they are provided by environmental package if relevant
</commit_message>
<xml_diff>
--- a/data/MIxS/Qiita_EBI_MIMS_v1.xlsx
+++ b/data/MIxS/Qiita_EBI_MIMS_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QiitaEBI" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>{term}</t>
   </si>
@@ -64,15 +64,6 @@
     <t>experimental_factor</t>
   </si>
   <si>
-    <t>depth</t>
-  </si>
-  <si>
-    <t>altitude</t>
-  </si>
-  <si>
-    <t>elevation</t>
-  </si>
-  <si>
     <t>geo_loc_name</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
   </si>
   <si>
     <t>{term, text}</t>
-  </si>
-  <si>
-    <t>{value} m</t>
   </si>
   <si>
     <t>M</t>
@@ -549,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -577,7 +565,7 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -586,7 +574,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -600,34 +588,34 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -650,16 +638,16 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -675,10 +663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -686,15 +674,14 @@
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -719,52 +706,34 @@
       <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -772,10 +741,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -784,18 +753,9 @@
         <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>